<commit_message>
added lockdown datasets, raw and filtered
</commit_message>
<xml_diff>
--- a/project datasets/covid_monthly_domesticviolence.xlsx
+++ b/project datasets/covid_monthly_domesticviolence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UNODC_projects\crime_data\output\portal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23be1045bd672b89/מסמכים/BGU/4th_semester/data_analysis/research/project datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13617466-BFFA-4988-947A-319CAE923B1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{13617466-BFFA-4988-947A-319CAE923B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90254C0E-E2AD-41CB-904D-E6ECA653F762}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="download_DomesticViolence.data" sheetId="1" r:id="rId1"/>
@@ -238,7 +238,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -777,33 +777,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O130" totalsRowShown="0">
-  <autoFilter ref="A1:O130"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O130" totalsRowShown="0">
+  <autoFilter ref="A1:O130" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Sexual violence or physical assault by IPFM*  (domestic violence): Total number of offences"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="15">
-    <tableColumn id="1" name="Region"/>
-    <tableColumn id="2" name="Sub region"/>
-    <tableColumn id="3" name="Country"/>
-    <tableColumn id="4" name="Indicator"/>
-    <tableColumn id="5" name="Oct_2019"/>
-    <tableColumn id="6" name="Nov_2019"/>
-    <tableColumn id="7" name="Dec_2019"/>
-    <tableColumn id="8" name="Jan_2020"/>
-    <tableColumn id="9" name="Feb_2020"/>
-    <tableColumn id="10" name="Mar_2020"/>
-    <tableColumn id="11" name="Apr_2020"/>
-    <tableColumn id="12" name="May_2020"/>
-    <tableColumn id="13" name="Jun_2020"/>
-    <tableColumn id="14" name="Jul_2020"/>
-    <tableColumn id="15" name="Aug_2020"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Region"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Sub region"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Country"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Indicator"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Oct_2019"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nov_2019"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Dec_2019"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Jan_2020"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Feb_2020"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Mar_2020"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Apr_2020"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="May_2020"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Jun_2020"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Jul_2020"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Aug_2020"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -841,7 +847,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -947,7 +953,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1089,39 +1095,39 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O130"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" customWidth="1"/>
+    <col min="8" max="8" width="10.54296875" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" customWidth="1"/>
+    <col min="11" max="11" width="10.6328125" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" customWidth="1"/>
+    <col min="13" max="13" width="10.54296875" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
-    <col min="15" max="15" width="10.88671875" customWidth="1"/>
+    <col min="15" max="15" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1168,7 +1174,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1215,7 +1221,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1247,7 +1253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1282,7 +1288,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1317,7 +1323,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1352,7 +1358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1387,7 +1393,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1422,7 +1428,7 @@
         <v>7776</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1457,7 +1463,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1492,7 +1498,7 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1539,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1586,7 +1592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1633,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1680,7 +1686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1709,7 +1715,7 @@
         <v>7289</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1738,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1767,7 +1773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1796,7 +1802,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1825,7 +1831,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1872,7 +1878,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1919,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1966,7 +1972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -2013,7 +2019,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -2060,7 +2066,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -2092,7 +2098,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -2124,7 +2130,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -2156,7 +2162,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -2188,7 +2194,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -2220,7 +2226,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -2240,7 +2246,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -2287,7 +2293,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -2334,7 +2340,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -2381,7 +2387,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -2428,7 +2434,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -2460,7 +2466,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -2504,7 +2510,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -2548,7 +2554,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -2595,7 +2601,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -2621,7 +2627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -2647,7 +2653,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -2694,7 +2700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -2741,7 +2747,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -2776,7 +2782,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -2811,7 +2817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -2846,7 +2852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -2881,7 +2887,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -2916,7 +2922,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -2963,7 +2969,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>15</v>
       </c>
@@ -3010,7 +3016,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -3057,7 +3063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -3104,7 +3110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -3151,7 +3157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -3198,7 +3204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>28</v>
       </c>
@@ -3242,7 +3248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>28</v>
       </c>
@@ -3265,7 +3271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -3312,7 +3318,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>15</v>
       </c>
@@ -3359,7 +3365,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -3376,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -3420,7 +3426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -3467,7 +3473,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>15</v>
       </c>
@@ -3514,7 +3520,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>28</v>
       </c>
@@ -3549,7 +3555,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>28</v>
       </c>
@@ -3584,7 +3590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>28</v>
       </c>
@@ -3619,7 +3625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>28</v>
       </c>
@@ -3654,7 +3660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>28</v>
       </c>
@@ -3689,7 +3695,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>28</v>
       </c>
@@ -3736,7 +3742,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>28</v>
       </c>
@@ -3783,7 +3789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>28</v>
       </c>
@@ -3830,7 +3836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>28</v>
       </c>
@@ -3877,7 +3883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -3924,7 +3930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>28</v>
       </c>
@@ -3971,7 +3977,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>28</v>
       </c>
@@ -4018,7 +4024,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>36</v>
       </c>
@@ -4065,7 +4071,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>36</v>
       </c>
@@ -4112,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>36</v>
       </c>
@@ -4159,7 +4165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>36</v>
       </c>
@@ -4206,7 +4212,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>36</v>
       </c>
@@ -4253,7 +4259,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>55</v>
       </c>
@@ -4300,7 +4306,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>55</v>
       </c>
@@ -4347,7 +4353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>55</v>
       </c>
@@ -4394,7 +4400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>55</v>
       </c>
@@ -4441,7 +4447,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>55</v>
       </c>
@@ -4488,7 +4494,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>15</v>
       </c>
@@ -4511,7 +4517,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -4528,7 +4534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>15</v>
       </c>
@@ -4551,7 +4557,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>15</v>
       </c>
@@ -4574,7 +4580,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>19</v>
       </c>
@@ -4621,7 +4627,7 @@
         <v>7799</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>19</v>
       </c>
@@ -4668,7 +4674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>19</v>
       </c>
@@ -4715,7 +4721,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>15</v>
       </c>
@@ -4762,7 +4768,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>15</v>
       </c>
@@ -4809,7 +4815,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>15</v>
       </c>
@@ -4856,7 +4862,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>15</v>
       </c>
@@ -4903,7 +4909,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>15</v>
       </c>
@@ -4950,7 +4956,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>28</v>
       </c>
@@ -4985,7 +4991,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>28</v>
       </c>
@@ -5020,7 +5026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>28</v>
       </c>
@@ -5055,7 +5061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>28</v>
       </c>
@@ -5090,7 +5096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>28</v>
       </c>
@@ -5125,7 +5131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>28</v>
       </c>
@@ -5160,7 +5166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>15</v>
       </c>
@@ -5192,7 +5198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>15</v>
       </c>
@@ -5233,7 +5239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>15</v>
       </c>
@@ -5262,7 +5268,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>15</v>
       </c>
@@ -5291,7 +5297,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>15</v>
       </c>
@@ -5338,7 +5344,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>15</v>
       </c>
@@ -5385,7 +5391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>15</v>
       </c>
@@ -5432,7 +5438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>15</v>
       </c>
@@ -5479,7 +5485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>15</v>
       </c>
@@ -5526,7 +5532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>15</v>
       </c>
@@ -5573,7 +5579,7 @@
         <v>9056</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>15</v>
       </c>
@@ -5620,7 +5626,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>15</v>
       </c>
@@ -5667,7 +5673,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>15</v>
       </c>
@@ -5714,7 +5720,7 @@
         <v>1586</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>15</v>
       </c>
@@ -5761,7 +5767,7 @@
         <v>7300</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>15</v>
       </c>
@@ -5805,7 +5811,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>15</v>
       </c>
@@ -5849,7 +5855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>15</v>
       </c>
@@ -5893,7 +5899,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>15</v>
       </c>
@@ -5937,7 +5943,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>15</v>
       </c>
@@ -5981,7 +5987,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>19</v>
       </c>
@@ -6016,7 +6022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>19</v>
       </c>
@@ -6051,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>19</v>
       </c>
@@ -6086,7 +6092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>19</v>
       </c>
@@ -6121,7 +6127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>19</v>
       </c>
@@ -6156,7 +6162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>19</v>
       </c>
@@ -6203,7 +6209,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>19</v>
       </c>
@@ -6250,7 +6256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>19</v>
       </c>
@@ -6297,7 +6303,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>28</v>
       </c>
@@ -6329,7 +6335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
added new data for us to use
</commit_message>
<xml_diff>
--- a/project datasets/covid_monthly_domesticviolence.xlsx
+++ b/project datasets/covid_monthly_domesticviolence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23be1045bd672b89/מסמכים/BGU/4th_semester/data_analysis/research/project datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{13617466-BFFA-4988-947A-319CAE923B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90254C0E-E2AD-41CB-904D-E6ECA653F762}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{13617466-BFFA-4988-947A-319CAE923B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7BE801E-7A94-404C-9E52-DE70D0DD36B2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="2460" windowWidth="14530" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="download_DomesticViolence.data" sheetId="1" r:id="rId1"/>
@@ -776,15 +776,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O130" totalsRowShown="0">
-  <autoFilter ref="A1:O130" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Sexual violence or physical assault by IPFM*  (domestic violence): Total number of offences"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:O130" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Region"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Sub region"/>
@@ -1105,7 +1103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1221,7 +1219,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1253,7 +1251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1323,7 +1321,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1358,7 +1356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1428,7 +1426,7 @@
         <v>7776</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1463,7 +1461,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1498,7 +1496,7 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1545,7 +1543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1592,7 +1590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1639,7 +1637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1715,7 +1713,7 @@
         <v>7289</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1744,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1773,7 +1771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1802,7 +1800,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1878,7 +1876,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1925,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -1972,7 +1970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -2019,7 +2017,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -2098,7 +2096,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -2130,7 +2128,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -2162,7 +2160,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -2194,7 +2192,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -2246,7 +2244,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -2293,7 +2291,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -2340,7 +2338,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -2387,7 +2385,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -2434,7 +2432,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -2466,7 +2464,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>15</v>
       </c>
@@ -2601,7 +2599,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -2627,7 +2625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -2653,7 +2651,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -2700,7 +2698,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -2782,7 +2780,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -2817,7 +2815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -2852,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -2887,7 +2885,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -3016,7 +3014,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>15</v>
       </c>
@@ -3063,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -3110,7 +3108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>15</v>
       </c>
@@ -3157,7 +3155,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -3248,7 +3246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>28</v>
       </c>
@@ -3271,7 +3269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>15</v>
       </c>
@@ -3365,7 +3363,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -3382,7 +3380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>15</v>
       </c>
@@ -3426,7 +3424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -3473,7 +3471,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>15</v>
       </c>
@@ -3555,7 +3553,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>28</v>
       </c>
@@ -3590,7 +3588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>28</v>
       </c>
@@ -3625,7 +3623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>28</v>
       </c>
@@ -3660,7 +3658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>28</v>
       </c>
@@ -3742,7 +3740,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>28</v>
       </c>
@@ -3789,7 +3787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>28</v>
       </c>
@@ -3836,7 +3834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>28</v>
       </c>
@@ -3883,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -3977,7 +3975,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>28</v>
       </c>
@@ -4071,7 +4069,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>36</v>
       </c>
@@ -4118,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>36</v>
       </c>
@@ -4165,7 +4163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>36</v>
       </c>
@@ -4212,7 +4210,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>36</v>
       </c>
@@ -4306,7 +4304,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>55</v>
       </c>
@@ -4353,7 +4351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>55</v>
       </c>
@@ -4400,7 +4398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>55</v>
       </c>
@@ -4447,7 +4445,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>55</v>
       </c>
@@ -4517,7 +4515,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -4534,7 +4532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>15</v>
       </c>
@@ -4557,7 +4555,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>15</v>
       </c>
@@ -4627,7 +4625,7 @@
         <v>7799</v>
       </c>
     </row>
-    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>19</v>
       </c>
@@ -4674,7 +4672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>19</v>
       </c>
@@ -4768,7 +4766,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>15</v>
       </c>
@@ -4815,7 +4813,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>15</v>
       </c>
@@ -4862,7 +4860,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>15</v>
       </c>
@@ -4909,7 +4907,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>15</v>
       </c>
@@ -4956,7 +4954,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>28</v>
       </c>
@@ -5026,7 +5024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>28</v>
       </c>
@@ -5061,7 +5059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>28</v>
       </c>
@@ -5096,7 +5094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>28</v>
       </c>
@@ -5131,7 +5129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>28</v>
       </c>
@@ -5166,7 +5164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>15</v>
       </c>
@@ -5198,7 +5196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>15</v>
       </c>
@@ -5239,7 +5237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>15</v>
       </c>
@@ -5268,7 +5266,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>15</v>
       </c>
@@ -5344,7 +5342,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>15</v>
       </c>
@@ -5391,7 +5389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>15</v>
       </c>
@@ -5438,7 +5436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>15</v>
       </c>
@@ -5485,7 +5483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>15</v>
       </c>
@@ -5579,7 +5577,7 @@
         <v>9056</v>
       </c>
     </row>
-    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>15</v>
       </c>
@@ -5626,7 +5624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>15</v>
       </c>
@@ -5673,7 +5671,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>15</v>
       </c>
@@ -5720,7 +5718,7 @@
         <v>1586</v>
       </c>
     </row>
-    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>15</v>
       </c>
@@ -5811,7 +5809,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>15</v>
       </c>
@@ -5855,7 +5853,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>15</v>
       </c>
@@ -5899,7 +5897,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>15</v>
       </c>
@@ -5943,7 +5941,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>15</v>
       </c>
@@ -5987,7 +5985,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>19</v>
       </c>
@@ -6022,7 +6020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>19</v>
       </c>
@@ -6057,7 +6055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>19</v>
       </c>
@@ -6092,7 +6090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>19</v>
       </c>
@@ -6127,7 +6125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>19</v>
       </c>
@@ -6209,7 +6207,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="127" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>19</v>
       </c>
@@ -6256,7 +6254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>19</v>
       </c>
@@ -6303,7 +6301,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>28</v>
       </c>
@@ -6335,7 +6333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>28</v>
       </c>

</xml_diff>